<commit_message>
Adding some more unit tests.
</commit_message>
<xml_diff>
--- a/pacehrh/tests/simple_config/Population Rates Test Data.xlsx
+++ b/pacehrh/tests/simple_config/Population Rates Test Data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlesel\Source\Ethiopia-HEP-Capacity-Analysis\ehep\tests\simple_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlesel\Source\Ethiopia-HEP-Capacity-Analysis\pacehrh\tests\simple_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C30C1A-B9F8-4029-8CAF-3D0C38047A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E213F99-DE50-44C6-B7E6-E8CDE0FDDEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="830" activeTab="1" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="830" activeTab="4" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="newPopValues" sheetId="84" r:id="rId1"/>
     <sheet name="badPopValues" sheetId="85" r:id="rId2"/>
     <sheet name="badPopValues_2" sheetId="86" r:id="rId3"/>
     <sheet name="badPopValues_3" sheetId="87" r:id="rId4"/>
+    <sheet name="badPopValues_4" sheetId="88" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="hours">#REF!</definedName>
@@ -147,8 +148,26 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={568A8AFA-191A-4450-82FD-7183877BD53F}</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{568A8AFA-191A-4450-82FD-7183877BD53F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Incomplete band - should go from 0-100</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -596,7 +615,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Scenarios_retain"/>
@@ -735,7 +754,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="To Do or Upgrade"/>
@@ -859,105 +878,6 @@
         <row r="77">
           <cell r="A77" t="str">
             <v>Ethiopia</v>
-          </cell>
-          <cell r="B77" t="str">
-            <v>ETH</v>
-          </cell>
-          <cell r="C77" t="str">
-            <v>Incidence of HIV, ages 15-49 (per 1,000 uninfected population ages 15-49)</v>
-          </cell>
-          <cell r="D77" t="str">
-            <v>SH.HIV.INCD.ZS</v>
-          </cell>
-          <cell r="AI77">
-            <v>5.58</v>
-          </cell>
-          <cell r="AJ77">
-            <v>5.77</v>
-          </cell>
-          <cell r="AK77">
-            <v>5.57</v>
-          </cell>
-          <cell r="AL77">
-            <v>4.9400000000000004</v>
-          </cell>
-          <cell r="AM77">
-            <v>4.09</v>
-          </cell>
-          <cell r="AN77">
-            <v>3.33</v>
-          </cell>
-          <cell r="AO77">
-            <v>2.72</v>
-          </cell>
-          <cell r="AP77">
-            <v>2.29</v>
-          </cell>
-          <cell r="AQ77">
-            <v>1.96</v>
-          </cell>
-          <cell r="AR77">
-            <v>1.65</v>
-          </cell>
-          <cell r="AS77">
-            <v>1.45</v>
-          </cell>
-          <cell r="AT77">
-            <v>1.26</v>
-          </cell>
-          <cell r="AU77">
-            <v>1.1399999999999999</v>
-          </cell>
-          <cell r="AV77">
-            <v>0.99</v>
-          </cell>
-          <cell r="AW77">
-            <v>0.92</v>
-          </cell>
-          <cell r="AX77">
-            <v>0.8</v>
-          </cell>
-          <cell r="AY77">
-            <v>0.75</v>
-          </cell>
-          <cell r="AZ77">
-            <v>0.7</v>
-          </cell>
-          <cell r="BA77">
-            <v>0.63</v>
-          </cell>
-          <cell r="BB77">
-            <v>0.59</v>
-          </cell>
-          <cell r="BC77">
-            <v>0.54</v>
-          </cell>
-          <cell r="BD77">
-            <v>0.49</v>
-          </cell>
-          <cell r="BE77">
-            <v>0.45</v>
-          </cell>
-          <cell r="BF77">
-            <v>0.38</v>
-          </cell>
-          <cell r="BG77">
-            <v>0.35</v>
-          </cell>
-          <cell r="BH77">
-            <v>0.32</v>
-          </cell>
-          <cell r="BI77">
-            <v>0.28999999999999998</v>
-          </cell>
-          <cell r="BJ77">
-            <v>0.27</v>
-          </cell>
-          <cell r="BK77">
-            <v>0.25</v>
-          </cell>
-          <cell r="BL77">
-            <v>0.23</v>
           </cell>
         </row>
       </sheetData>
@@ -1316,6 +1236,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E2" dT="2023-05-25T23:11:08.63" personId="{7F693746-57BF-47BE-B765-B7B04423F821}" id="{568A8AFA-191A-4450-82FD-7183877BD53F}">
+    <text>Incomplete band - should go from 0-100</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E7F677-BE8D-4B15-BFBB-F131739569D4}">
   <dimension ref="A1:I31"/>
@@ -1324,19 +1252,19 @@
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +1293,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1385,7 +1313,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1408,7 +1336,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1437,7 +1365,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1466,7 +1394,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1495,7 +1423,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1524,7 +1452,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1553,7 +1481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1510,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1611,7 +1539,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1634,7 +1562,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1660,7 +1588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1689,7 +1617,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1718,7 +1646,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1747,7 +1675,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1776,7 +1704,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1805,7 +1733,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1834,7 +1762,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1863,7 +1791,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1892,7 +1820,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1918,7 +1846,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -1944,7 +1872,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1973,7 +1901,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2002,7 +1930,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -2031,7 +1959,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -2060,7 +1988,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -2089,7 +2017,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2118,7 +2046,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2147,7 +2075,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -2176,7 +2104,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2211,23 +2139,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11567A4-E3D5-48A5-8F95-3D034A772443}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2256,7 +2184,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -2276,7 +2204,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2299,7 +2227,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2328,7 +2256,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2357,7 +2285,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2386,7 +2314,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2415,7 +2343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2444,7 +2372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2473,7 +2401,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2502,7 +2430,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2525,7 +2453,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2551,7 +2479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -2580,7 +2508,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2609,7 +2537,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2638,7 +2566,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2667,7 +2595,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -2696,7 +2624,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2725,7 +2653,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2754,7 +2682,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2783,7 +2711,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2812,7 +2740,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -2838,7 +2766,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2867,7 +2795,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2896,7 +2824,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -2925,7 +2853,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -2954,7 +2882,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -2983,7 +2911,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -3012,7 +2940,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -3041,7 +2969,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -3070,7 +2998,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -3110,19 +3038,19 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3151,7 +3079,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -3171,7 +3099,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -3194,7 +3122,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3223,7 +3151,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3252,7 +3180,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3281,7 +3209,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3310,7 +3238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3339,7 +3267,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3368,7 +3296,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -3397,7 +3325,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -3420,7 +3348,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -3446,7 +3374,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -3475,7 +3403,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3504,7 +3432,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -3533,7 +3461,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -3562,7 +3490,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -3591,7 +3519,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3620,7 +3548,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -3649,7 +3577,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3678,7 +3606,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -3707,7 +3635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -3733,7 +3661,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -3762,7 +3690,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -3791,7 +3719,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -3820,7 +3748,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -3849,7 +3777,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -3878,7 +3806,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -3907,7 +3835,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -3936,7 +3864,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -3965,7 +3893,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -4005,19 +3933,19 @@
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4046,7 +3974,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -4066,7 +3994,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -4089,7 +4017,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4118,7 +4046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4147,7 +4075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -4176,7 +4104,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4205,7 +4133,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4234,7 +4162,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4263,7 +4191,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4292,7 +4220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -4315,7 +4243,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -4341,7 +4269,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -4370,7 +4298,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -4399,7 +4327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -4428,7 +4356,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -4457,7 +4385,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -4486,7 +4414,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -4515,7 +4443,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -4544,7 +4472,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -4573,7 +4501,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -4599,7 +4527,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -4625,7 +4553,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -4654,7 +4582,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -4683,7 +4611,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -4712,7 +4640,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -4741,7 +4669,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -4770,7 +4698,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -4799,7 +4727,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -4828,7 +4756,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -4857,7 +4785,905 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>75</v>
+      </c>
+      <c r="G31">
+        <v>0.10501017502993976</v>
+      </c>
+      <c r="H31">
+        <v>0.98481071022469158</v>
+      </c>
+      <c r="I31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142B2228-AFC4-4F56-B519-7BBCBB207093}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>98</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H4">
+        <v>0.98846927759109204</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.99316389691241536</v>
+      </c>
+      <c r="I5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="H6">
+        <v>0.98022410443373342</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.97771923789514636</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>39</v>
+      </c>
+      <c r="G8">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.97393215219000295</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="H9">
+        <v>0.95811661983967134</v>
+      </c>
+      <c r="I9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>49</v>
+      </c>
+      <c r="G10">
+        <v>1.4E-2</v>
+      </c>
+      <c r="H10">
+        <v>0.91700404320467122</v>
+      </c>
+      <c r="I10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>4.4870649522800003E-2</v>
+      </c>
+      <c r="H12">
+        <v>0.96306068601583117</v>
+      </c>
+      <c r="I12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>3.5500000000000006E-3</v>
+      </c>
+      <c r="H13">
+        <v>0.95480225988700573</v>
+      </c>
+      <c r="I13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>1.1800000000000001E-3</v>
+      </c>
+      <c r="H14">
+        <v>0.95161290322580649</v>
+      </c>
+      <c r="I14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>9.5999999999999992E-4</v>
+      </c>
+      <c r="H15">
+        <v>0.96150047483380818</v>
+      </c>
+      <c r="I15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>19</v>
+      </c>
+      <c r="G16">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H16">
+        <v>0.96508794519599173</v>
+      </c>
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <v>1.72E-3</v>
+      </c>
+      <c r="H17">
+        <v>0.9885057471264368</v>
+      </c>
+      <c r="I17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>35</v>
+      </c>
+      <c r="F18">
+        <v>49</v>
+      </c>
+      <c r="G18">
+        <v>4.6410387643786967E-3</v>
+      </c>
+      <c r="H18">
+        <v>0.98007627674588871</v>
+      </c>
+      <c r="I18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>50</v>
+      </c>
+      <c r="F19">
+        <v>59</v>
+      </c>
+      <c r="G19">
+        <v>7.8897658994437833E-3</v>
+      </c>
+      <c r="H19">
+        <v>0.98007627674588871</v>
+      </c>
+      <c r="I19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>60</v>
+      </c>
+      <c r="F20">
+        <v>74</v>
+      </c>
+      <c r="G20">
+        <v>2.2091344518442593E-2</v>
+      </c>
+      <c r="H20">
+        <v>0.98007627674588871</v>
+      </c>
+      <c r="I20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>75</v>
+      </c>
+      <c r="G21">
+        <v>8.6787424893881623E-2</v>
+      </c>
+      <c r="H21">
+        <v>0.98007627674588871</v>
+      </c>
+      <c r="I21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>4.4870649522800003E-2</v>
+      </c>
+      <c r="H22">
+        <v>0.96306068601583117</v>
+      </c>
+      <c r="I22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>3.5500000000000006E-3</v>
+      </c>
+      <c r="H23">
+        <v>0.95480225988700573</v>
+      </c>
+      <c r="I23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>1.1800000000000001E-3</v>
+      </c>
+      <c r="H24">
+        <v>0.95161290322580649</v>
+      </c>
+      <c r="I24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>9.5999999999999992E-4</v>
+      </c>
+      <c r="H25">
+        <v>0.96150047483380818</v>
+      </c>
+      <c r="I25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>19</v>
+      </c>
+      <c r="G26">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H26">
+        <v>0.96508794519599173</v>
+      </c>
+      <c r="I26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>34</v>
+      </c>
+      <c r="G27">
+        <v>1.72E-3</v>
+      </c>
+      <c r="H27">
+        <v>0.9885057471264368</v>
+      </c>
+      <c r="I27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>35</v>
+      </c>
+      <c r="F28">
+        <v>49</v>
+      </c>
+      <c r="G28">
+        <v>6.3527026636382199E-3</v>
+      </c>
+      <c r="H28">
+        <v>0.98481071022469158</v>
+      </c>
+      <c r="I28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>50</v>
+      </c>
+      <c r="F29">
+        <v>59</v>
+      </c>
+      <c r="G29">
+        <v>1.2070135060912618E-2</v>
+      </c>
+      <c r="H29">
+        <v>0.98481071022469158</v>
+      </c>
+      <c r="I29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>60</v>
+      </c>
+      <c r="F30">
+        <v>74</v>
+      </c>
+      <c r="G30">
+        <v>3.1382351158372804E-2</v>
+      </c>
+      <c r="H30">
+        <v>0.98481071022469158</v>
+      </c>
+      <c r="I30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>19</v>
       </c>

</xml_diff>